<commit_message>
Poprawa bazy i pustych komórek
</commit_message>
<xml_diff>
--- a/Backend/baza.xlsx
+++ b/Backend/baza.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
   <si>
     <t>nazwa imprezy/wydarzenia</t>
   </si>
@@ -333,9 +333,6 @@
   </si>
   <si>
     <t>Oddział PTTK Tryton w Nysie/Stowarzyszenie Miłośników Kolei Racławice Śląskie/ Informacja Turystyczna</t>
-  </si>
-  <si>
-    <t>wg odrębnego programu</t>
   </si>
   <si>
     <t>27.11.2017</t>
@@ -556,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -585,29 +582,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +909,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -927,7 +930,7 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -944,7 +947,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="13"/>
       <c r="D5" s="15"/>
       <c r="E5" s="4" t="s">
@@ -953,7 +956,7 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -970,7 +973,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="13"/>
       <c r="D7" s="15"/>
       <c r="E7" s="4" t="s">
@@ -1192,7 +1195,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -1209,7 +1212,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="13"/>
       <c r="D22" s="4" t="s">
         <v>58</v>
@@ -1218,7 +1221,7 @@
       <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="12" t="s">
@@ -1230,21 +1233,19 @@
       <c r="E23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="17"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="13"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -1256,18 +1257,16 @@
       <c r="E25" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="17"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="13"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F26" s="19"/>
     </row>
     <row r="27" spans="2:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
@@ -1299,7 +1298,9 @@
       <c r="E28" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="29" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
@@ -1396,7 +1397,7 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -1413,7 +1414,7 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="17"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="13"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
@@ -1540,8 +1541,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
+    <row r="44" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="16" t="s">
         <v>99</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -1553,25 +1554,23 @@
       <c r="E44" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="18" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="11"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="13"/>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
-      <c r="F45" s="8" t="s">
-        <v>103</v>
-      </c>
+      <c r="F45" s="19"/>
     </row>
     <row r="46" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>27</v>
@@ -1583,10 +1582,10 @@
     </row>
     <row r="47" spans="2:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>13</v>
@@ -1595,15 +1594,15 @@
         <v>24</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>13</v>
@@ -1617,27 +1616,27 @@
     </row>
     <row r="49" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E49" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F49" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>13</v>
@@ -1654,7 +1653,7 @@
         <v>33</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>7</v>
@@ -1668,16 +1667,16 @@
     </row>
     <row r="52" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>16</v>
@@ -1685,10 +1684,10 @@
     </row>
     <row r="53" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>13</v>
@@ -1701,23 +1700,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
+  <mergeCells count="31">
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F44:F45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="D44:D45"/>
@@ -1730,6 +1715,23 @@
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="E35:E36"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tym razem legitna baza
</commit_message>
<xml_diff>
--- a/Backend/baza.xlsx
+++ b/Backend/baza.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="122">
   <si>
     <t>nazwa imprezy/wydarzenia</t>
   </si>
@@ -582,35 +582,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,56 +930,56 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="15"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="15"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
@@ -1045,7 +1045,9 @@
       <c r="E11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
@@ -1071,7 +1073,9 @@
       <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="E13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1137,7 +1141,9 @@
       <c r="C17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="E17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1192,81 +1198,83 @@
       <c r="E20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
-      <c r="C22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="2:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
@@ -1309,11 +1317,15 @@
       <c r="C29" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="E29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="8"/>
+      <c r="F29" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="30" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
@@ -1339,7 +1351,9 @@
       <c r="C31" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="E31" s="4" t="s">
         <v>24</v>
       </c>
@@ -1397,16 +1411,16 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="16" t="s">
         <v>86</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -1414,10 +1428,10 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="11"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="8" t="s">
         <v>61</v>
       </c>
@@ -1542,28 +1556,28 @@
       </c>
     </row>
     <row r="44" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="17"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="19"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
@@ -1578,7 +1592,9 @@
       <c r="E46" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="8"/>
+      <c r="F46" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="47" spans="2:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6" t="s">
@@ -1701,6 +1717,23 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F44:F45"/>
     <mergeCell ref="B44:B45"/>
@@ -1715,23 +1748,6 @@
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="E35:E36"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>